<commit_message>
Migrate to New Backend/Sheet (New URL)
</commit_message>
<xml_diff>
--- a/QRFINAL/INVENTARIO OFICIAL BODEGA MANTENCION CERMAQ.xlsx
+++ b/QRFINAL/INVENTARIO OFICIAL BODEGA MANTENCION CERMAQ.xlsx
@@ -255,38 +255,41 @@
   <dxfs count="20">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <color auto="1"/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -327,38 +330,41 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <color auto="1"/>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -399,6 +405,44 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -435,6 +479,44 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -467,6 +549,192 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -530,282 +798,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD8D8D8"/>
@@ -829,13 +821,21 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="2026-style" pivot="0" count="4">
       <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="secondRowStripe" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -854,15 +854,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:G1001" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:G1001" totalsRowShown="0" dataDxfId="14">
   <tableColumns count="7">
-    <tableColumn id="1" name="N° ARTICULO" dataDxfId="6" totalsRowDxfId="15"/>
-    <tableColumn id="2" name="DESCRIPCION DEL ARTICULO" dataDxfId="5" totalsRowDxfId="14"/>
-    <tableColumn id="3" name="UNI. MEDIDA" dataDxfId="4" totalsRowDxfId="13"/>
-    <tableColumn id="4" name="STOCK" dataDxfId="3" totalsRowDxfId="12"/>
-    <tableColumn id="5" name="CATEGORIA" dataDxfId="2" totalsRowDxfId="11"/>
-    <tableColumn id="6" name="PRECIO" dataDxfId="1" totalsRowDxfId="10"/>
-    <tableColumn id="7" name="PRECIO SEGÚN STOCK" dataDxfId="0" totalsRowDxfId="9"/>
+    <tableColumn id="1" name="N° ARTICULO" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" name="DESCRIPCION DEL ARTICULO" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="UNI. MEDIDA" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="STOCK" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="CATEGORIA" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="PRECIO" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" name="PRECIO SEGÚN STOCK" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="2026-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1068,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A879" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13165,7 +13165,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:Z2">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13185,7 +13185,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13288,7 +13288,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1048538" sqref="K1048538"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>